<commit_message>
nhcuong: Unify MySEvent to MyEvent + Maintain code
</commit_message>
<xml_diff>
--- a/doc/0512082_0512085_0512121_PhieuDanhGia.xlsx
+++ b/doc/0512082_0512085_0512121_PhieuDanhGia.xlsx
@@ -735,7 +735,7 @@
   <dimension ref="A1:I66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1139,7 +1139,9 @@
       <c r="C25" s="21">
         <v>0.25</v>
       </c>
-      <c r="D25" s="23"/>
+      <c r="D25" s="23">
+        <v>0.25</v>
+      </c>
       <c r="E25" s="23"/>
       <c r="F25" s="23"/>
     </row>
@@ -1300,7 +1302,9 @@
       <c r="C36" s="21">
         <v>0.25</v>
       </c>
-      <c r="D36" s="23"/>
+      <c r="D36" s="23">
+        <v>0.25</v>
+      </c>
       <c r="E36" s="23"/>
       <c r="F36" s="23"/>
       <c r="I36" s="2"/>
@@ -1421,7 +1425,7 @@
       </c>
       <c r="D44" s="25">
         <f>SUM(D9:D43)</f>
-        <v>3.75</v>
+        <v>4.25</v>
       </c>
       <c r="E44" s="25">
         <f>SUM(E9:E43)</f>

</xml_diff>

<commit_message>
nhcuong: update path separator
</commit_message>
<xml_diff>
--- a/doc/0512082_0512085_0512121_PhieuDanhGia.xlsx
+++ b/doc/0512082_0512085_0512121_PhieuDanhGia.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="67">
   <si>
     <t>STT</t>
   </si>
@@ -205,30 +205,6 @@
   </si>
   <si>
     <t>Tự đánh giá khống (Chức năng không làm mà đánh giá)</t>
-  </si>
-  <si>
-    <t>chưa làm trực tiếp trên form</t>
-  </si>
-  <si>
-    <t>không cho phép thực hiện trên thư mục</t>
-  </si>
-  <si>
-    <t>delete multi files</t>
-  </si>
-  <si>
-    <t>copy multi files</t>
-  </si>
-  <si>
-    <t>move multi files</t>
-  </si>
-  <si>
-    <t>delete multi folders</t>
-  </si>
-  <si>
-    <t>copy multi folders</t>
-  </si>
-  <si>
-    <t>move multi folders</t>
   </si>
   <si>
     <t>Phạm Minh Chánh</t>
@@ -734,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10:F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -795,7 +771,7 @@
         <v>512082</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -809,12 +785,12 @@
         <v>512085</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="4" customFormat="1">
@@ -825,7 +801,7 @@
         <v>512121</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
@@ -889,9 +865,7 @@
         <v>0.25</v>
       </c>
       <c r="E10" s="14"/>
-      <c r="F10" s="14" t="s">
-        <v>64</v>
-      </c>
+      <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="12">
@@ -907,9 +881,7 @@
         <v>0.25</v>
       </c>
       <c r="E11" s="14"/>
-      <c r="F11" s="14" t="s">
-        <v>63</v>
-      </c>
+      <c r="F11" s="14"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="12">
@@ -925,9 +897,7 @@
         <v>0.25</v>
       </c>
       <c r="E12" s="14"/>
-      <c r="F12" s="14" t="s">
-        <v>65</v>
-      </c>
+      <c r="F12" s="14"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="12">
@@ -943,9 +913,7 @@
         <v>0.25</v>
       </c>
       <c r="E13" s="14"/>
-      <c r="F13" s="14" t="s">
-        <v>66</v>
-      </c>
+      <c r="F13" s="14"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="12">
@@ -961,9 +929,7 @@
         <v>0.25</v>
       </c>
       <c r="E14" s="14"/>
-      <c r="F14" s="14" t="s">
-        <v>67</v>
-      </c>
+      <c r="F14" s="14"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="12">
@@ -979,9 +945,7 @@
         <v>0.25</v>
       </c>
       <c r="E15" s="14"/>
-      <c r="F15" s="14" t="s">
-        <v>64</v>
-      </c>
+      <c r="F15" s="14"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="18">
@@ -1013,9 +977,7 @@
         <v>0.25</v>
       </c>
       <c r="E17" s="20"/>
-      <c r="F17" s="20" t="s">
-        <v>63</v>
-      </c>
+      <c r="F17" s="20"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="18">
@@ -1031,9 +993,7 @@
         <v>0.25</v>
       </c>
       <c r="E18" s="20"/>
-      <c r="F18" s="20" t="s">
-        <v>68</v>
-      </c>
+      <c r="F18" s="20"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="18">
@@ -1049,9 +1009,7 @@
         <v>0.25</v>
       </c>
       <c r="E19" s="20"/>
-      <c r="F19" s="20" t="s">
-        <v>69</v>
-      </c>
+      <c r="F19" s="20"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="18">
@@ -1067,9 +1025,7 @@
         <v>0.25</v>
       </c>
       <c r="E20" s="20"/>
-      <c r="F20" s="20" t="s">
-        <v>70</v>
-      </c>
+      <c r="F20" s="20"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="21">

</xml_diff>

<commit_message>
nhcuong: Maintain code + coding convention
</commit_message>
<xml_diff>
--- a/doc/0512082_0512085_0512121_PhieuDanhGia.xlsx
+++ b/doc/0512082_0512085_0512121_PhieuDanhGia.xlsx
@@ -710,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1131,7 +1131,9 @@
       <c r="C27" s="15">
         <v>0.25</v>
       </c>
-      <c r="D27" s="17"/>
+      <c r="D27" s="17">
+        <v>0.25</v>
+      </c>
       <c r="E27" s="17"/>
       <c r="F27" s="17"/>
     </row>
@@ -1317,7 +1319,9 @@
       <c r="C39" s="21">
         <v>0.25</v>
       </c>
-      <c r="D39" s="23"/>
+      <c r="D39" s="23">
+        <v>0.25</v>
+      </c>
       <c r="E39" s="23"/>
       <c r="F39" s="23"/>
       <c r="G39" s="2"/>
@@ -1347,7 +1351,7 @@
       <c r="C41" s="21">
         <v>0.25</v>
       </c>
-      <c r="D41" s="24"/>
+      <c r="D41" s="22"/>
       <c r="E41" s="23"/>
       <c r="F41" s="23"/>
     </row>
@@ -1391,7 +1395,7 @@
       </c>
       <c r="D44" s="25">
         <f>SUM(D9:D43)</f>
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="E44" s="25">
         <f>SUM(E9:E43)</f>

</xml_diff>

<commit_message>
nhcuong: Relayout - round 5 - Zip and Unzip
</commit_message>
<xml_diff>
--- a/doc/0512082_0512085_0512121_PhieuDanhGia.xlsx
+++ b/doc/0512082_0512085_0512121_PhieuDanhGia.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="68">
   <si>
     <t>STT</t>
   </si>
@@ -217,6 +217,9 @@
   </si>
   <si>
     <t>Trịnh Trung Hiếu</t>
+  </si>
+  <si>
+    <t>ok</t>
   </si>
 </sst>
 </file>
@@ -711,7 +714,7 @@
   <dimension ref="A1:I66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -848,7 +851,9 @@
       <c r="D9" s="14">
         <v>0.25</v>
       </c>
-      <c r="E9" s="14"/>
+      <c r="E9" s="14" t="s">
+        <v>67</v>
+      </c>
       <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6">
@@ -864,7 +869,9 @@
       <c r="D10" s="14">
         <v>0.25</v>
       </c>
-      <c r="E10" s="14"/>
+      <c r="E10" s="14" t="s">
+        <v>67</v>
+      </c>
       <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:6">
@@ -880,7 +887,9 @@
       <c r="D11" s="14">
         <v>0.25</v>
       </c>
-      <c r="E11" s="14"/>
+      <c r="E11" s="14" t="s">
+        <v>67</v>
+      </c>
       <c r="F11" s="14"/>
     </row>
     <row r="12" spans="1:6">
@@ -896,7 +905,9 @@
       <c r="D12" s="14">
         <v>0.25</v>
       </c>
-      <c r="E12" s="14"/>
+      <c r="E12" s="14" t="s">
+        <v>67</v>
+      </c>
       <c r="F12" s="14"/>
     </row>
     <row r="13" spans="1:6">
@@ -912,7 +923,9 @@
       <c r="D13" s="14">
         <v>0.25</v>
       </c>
-      <c r="E13" s="14"/>
+      <c r="E13" s="14" t="s">
+        <v>67</v>
+      </c>
       <c r="F13" s="14"/>
     </row>
     <row r="14" spans="1:6">
@@ -928,7 +941,9 @@
       <c r="D14" s="14">
         <v>0.25</v>
       </c>
-      <c r="E14" s="14"/>
+      <c r="E14" s="14" t="s">
+        <v>67</v>
+      </c>
       <c r="F14" s="14"/>
     </row>
     <row r="15" spans="1:6">
@@ -944,7 +959,9 @@
       <c r="D15" s="14">
         <v>0.25</v>
       </c>
-      <c r="E15" s="14"/>
+      <c r="E15" s="14" t="s">
+        <v>67</v>
+      </c>
       <c r="F15" s="14"/>
     </row>
     <row r="16" spans="1:6">
@@ -960,7 +977,9 @@
       <c r="D16" s="20">
         <v>0.25</v>
       </c>
-      <c r="E16" s="20"/>
+      <c r="E16" s="20" t="s">
+        <v>67</v>
+      </c>
       <c r="F16" s="20"/>
     </row>
     <row r="17" spans="1:8">
@@ -976,7 +995,9 @@
       <c r="D17" s="20">
         <v>0.25</v>
       </c>
-      <c r="E17" s="20"/>
+      <c r="E17" s="20" t="s">
+        <v>67</v>
+      </c>
       <c r="F17" s="20"/>
     </row>
     <row r="18" spans="1:8">
@@ -992,7 +1013,9 @@
       <c r="D18" s="20">
         <v>0.25</v>
       </c>
-      <c r="E18" s="20"/>
+      <c r="E18" s="20" t="s">
+        <v>67</v>
+      </c>
       <c r="F18" s="20"/>
     </row>
     <row r="19" spans="1:8">
@@ -1008,7 +1031,9 @@
       <c r="D19" s="20">
         <v>0.25</v>
       </c>
-      <c r="E19" s="20"/>
+      <c r="E19" s="20" t="s">
+        <v>67</v>
+      </c>
       <c r="F19" s="20"/>
     </row>
     <row r="20" spans="1:8">
@@ -1024,7 +1049,9 @@
       <c r="D20" s="20">
         <v>0.25</v>
       </c>
-      <c r="E20" s="20"/>
+      <c r="E20" s="20" t="s">
+        <v>67</v>
+      </c>
       <c r="F20" s="20"/>
     </row>
     <row r="21" spans="1:8">

</xml_diff>

<commit_message>
nhcuong: Look and Feel (update)
</commit_message>
<xml_diff>
--- a/doc/0512082_0512085_0512121_PhieuDanhGia.xlsx
+++ b/doc/0512082_0512085_0512121_PhieuDanhGia.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="67">
   <si>
     <t>STT</t>
   </si>
@@ -217,9 +217,6 @@
   </si>
   <si>
     <t>Trịnh Trung Hiếu</t>
-  </si>
-  <si>
-    <t>ok</t>
   </si>
 </sst>
 </file>
@@ -713,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -851,9 +848,7 @@
       <c r="D9" s="14">
         <v>0.25</v>
       </c>
-      <c r="E9" s="14" t="s">
-        <v>67</v>
-      </c>
+      <c r="E9" s="14"/>
       <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6">
@@ -869,9 +864,7 @@
       <c r="D10" s="14">
         <v>0.25</v>
       </c>
-      <c r="E10" s="14" t="s">
-        <v>67</v>
-      </c>
+      <c r="E10" s="14"/>
       <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:6">
@@ -887,9 +880,7 @@
       <c r="D11" s="14">
         <v>0.25</v>
       </c>
-      <c r="E11" s="14" t="s">
-        <v>67</v>
-      </c>
+      <c r="E11" s="14"/>
       <c r="F11" s="14"/>
     </row>
     <row r="12" spans="1:6">
@@ -905,9 +896,7 @@
       <c r="D12" s="14">
         <v>0.25</v>
       </c>
-      <c r="E12" s="14" t="s">
-        <v>67</v>
-      </c>
+      <c r="E12" s="14"/>
       <c r="F12" s="14"/>
     </row>
     <row r="13" spans="1:6">
@@ -923,9 +912,7 @@
       <c r="D13" s="14">
         <v>0.25</v>
       </c>
-      <c r="E13" s="14" t="s">
-        <v>67</v>
-      </c>
+      <c r="E13" s="14"/>
       <c r="F13" s="14"/>
     </row>
     <row r="14" spans="1:6">
@@ -941,9 +928,7 @@
       <c r="D14" s="14">
         <v>0.25</v>
       </c>
-      <c r="E14" s="14" t="s">
-        <v>67</v>
-      </c>
+      <c r="E14" s="14"/>
       <c r="F14" s="14"/>
     </row>
     <row r="15" spans="1:6">
@@ -959,9 +944,7 @@
       <c r="D15" s="14">
         <v>0.25</v>
       </c>
-      <c r="E15" s="14" t="s">
-        <v>67</v>
-      </c>
+      <c r="E15" s="14"/>
       <c r="F15" s="14"/>
     </row>
     <row r="16" spans="1:6">
@@ -977,9 +960,7 @@
       <c r="D16" s="20">
         <v>0.25</v>
       </c>
-      <c r="E16" s="20" t="s">
-        <v>67</v>
-      </c>
+      <c r="E16" s="20"/>
       <c r="F16" s="20"/>
     </row>
     <row r="17" spans="1:8">
@@ -995,9 +976,7 @@
       <c r="D17" s="20">
         <v>0.25</v>
       </c>
-      <c r="E17" s="20" t="s">
-        <v>67</v>
-      </c>
+      <c r="E17" s="20"/>
       <c r="F17" s="20"/>
     </row>
     <row r="18" spans="1:8">
@@ -1013,9 +992,7 @@
       <c r="D18" s="20">
         <v>0.25</v>
       </c>
-      <c r="E18" s="20" t="s">
-        <v>67</v>
-      </c>
+      <c r="E18" s="20"/>
       <c r="F18" s="20"/>
     </row>
     <row r="19" spans="1:8">
@@ -1031,9 +1008,7 @@
       <c r="D19" s="20">
         <v>0.25</v>
       </c>
-      <c r="E19" s="20" t="s">
-        <v>67</v>
-      </c>
+      <c r="E19" s="20"/>
       <c r="F19" s="20"/>
     </row>
     <row r="20" spans="1:8">
@@ -1049,9 +1024,7 @@
       <c r="D20" s="20">
         <v>0.25</v>
       </c>
-      <c r="E20" s="20" t="s">
-        <v>67</v>
-      </c>
+      <c r="E20" s="20"/>
       <c r="F20" s="20"/>
     </row>
     <row r="21" spans="1:8">
@@ -1267,7 +1240,9 @@
       <c r="C34" s="21">
         <v>0.25</v>
       </c>
-      <c r="D34" s="23"/>
+      <c r="D34" s="23">
+        <v>0.25</v>
+      </c>
       <c r="E34" s="23"/>
       <c r="F34" s="23"/>
       <c r="H34" s="2"/>
@@ -1422,7 +1397,7 @@
       </c>
       <c r="D44" s="25">
         <f>SUM(D9:D43)</f>
-        <v>6</v>
+        <v>6.25</v>
       </c>
       <c r="E44" s="25">
         <f>SUM(E9:E43)</f>

</xml_diff>

<commit_message>
nhcuong: Relayout - finished!
</commit_message>
<xml_diff>
--- a/doc/0512082_0512085_0512121_PhieuDanhGia.xlsx
+++ b/doc/0512082_0512085_0512121_PhieuDanhGia.xlsx
@@ -710,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -773,7 +773,9 @@
       <c r="C4" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="10"/>
+      <c r="D4" s="10">
+        <v>100</v>
+      </c>
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
@@ -787,7 +789,9 @@
       <c r="C5" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="10"/>
+      <c r="D5" s="10">
+        <v>100</v>
+      </c>
       <c r="E5" s="10"/>
       <c r="F5" s="10" t="s">
         <v>65</v>
@@ -803,7 +807,9 @@
       <c r="C6" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="D6" s="10"/>
+      <c r="D6" s="10">
+        <v>100</v>
+      </c>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
     </row>

</xml_diff>